<commit_message>
Small ball fixes to tables.
</commit_message>
<xml_diff>
--- a/FOIA SAR data/JSF/JSF Dec 2013 SAR Data Draw.xlsx
+++ b/FOIA SAR data/JSF/JSF Dec 2013 SAR Data Draw.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\2015-09 Joint Development\Research\JSF F-35\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Greg Sanders\Documents\Development\R-scripts-and-data\FOIA SAR data\JSF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="CostSummary" sheetId="1" r:id="rId1"/>
@@ -1939,25 +1939,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1985,6 +1976,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2363,76 +2363,76 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="119"/>
-      <c r="B3" s="126" t="s">
+      <c r="A3" s="121"/>
+      <c r="B3" s="123" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="127"/>
+      <c r="C3" s="124"/>
       <c r="D3" s="31"/>
       <c r="E3" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F3" s="126" t="s">
+      <c r="F3" s="123" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="127"/>
-      <c r="H3" s="130"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="127"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="120"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="129"/>
+      <c r="A4" s="122"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="126"/>
       <c r="D4" s="32"/>
       <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="131"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="133"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="130"/>
     </row>
     <row r="5" spans="1:8" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="126" t="s">
+      <c r="C5" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="130"/>
-      <c r="E5" s="121" t="s">
+      <c r="D5" s="127"/>
+      <c r="E5" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="128"/>
-      <c r="G5" s="129"/>
-      <c r="H5" s="134"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="131"/>
     </row>
     <row r="6" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="124"/>
-      <c r="B6" s="122"/>
-      <c r="C6" s="131"/>
-      <c r="D6" s="133"/>
-      <c r="E6" s="124"/>
-      <c r="F6" s="121" t="s">
+      <c r="A6" s="132"/>
+      <c r="B6" s="134"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="121" t="s">
+      <c r="G6" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="121" t="s">
+      <c r="H6" s="119" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="125"/>
-      <c r="B7" s="123"/>
-      <c r="C7" s="128"/>
-      <c r="D7" s="134"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="125"/>
-      <c r="G7" s="125"/>
-      <c r="H7" s="125"/>
+      <c r="A7" s="133"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="125"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="133"/>
+      <c r="G7" s="133"/>
+      <c r="H7" s="133"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
@@ -2736,76 +2736,76 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="119"/>
-      <c r="B21" s="126" t="s">
+      <c r="A21" s="121"/>
+      <c r="B21" s="123" t="s">
         <v>166</v>
       </c>
-      <c r="C21" s="127"/>
+      <c r="C21" s="124"/>
       <c r="D21" s="31"/>
       <c r="E21" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F21" s="126" t="s">
+      <c r="F21" s="123" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="127"/>
-      <c r="H21" s="130"/>
+      <c r="G21" s="124"/>
+      <c r="H21" s="127"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="120"/>
-      <c r="B22" s="128"/>
-      <c r="C22" s="129"/>
+      <c r="A22" s="122"/>
+      <c r="B22" s="125"/>
+      <c r="C22" s="126"/>
       <c r="D22" s="32"/>
       <c r="E22" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="131"/>
-      <c r="G22" s="132"/>
-      <c r="H22" s="133"/>
+      <c r="F22" s="128"/>
+      <c r="G22" s="129"/>
+      <c r="H22" s="130"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="121" t="s">
+      <c r="A23" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="121" t="s">
+      <c r="B23" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="126" t="s">
+      <c r="C23" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="130"/>
-      <c r="E23" s="121" t="s">
+      <c r="D23" s="127"/>
+      <c r="E23" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="128"/>
-      <c r="G23" s="129"/>
-      <c r="H23" s="134"/>
+      <c r="F23" s="125"/>
+      <c r="G23" s="126"/>
+      <c r="H23" s="131"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="124"/>
-      <c r="B24" s="122"/>
-      <c r="C24" s="131"/>
-      <c r="D24" s="133"/>
-      <c r="E24" s="124"/>
-      <c r="F24" s="121" t="s">
+      <c r="A24" s="132"/>
+      <c r="B24" s="134"/>
+      <c r="C24" s="128"/>
+      <c r="D24" s="130"/>
+      <c r="E24" s="132"/>
+      <c r="F24" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="121" t="s">
+      <c r="G24" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="121" t="s">
+      <c r="H24" s="119" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="125"/>
-      <c r="B25" s="123"/>
-      <c r="C25" s="128"/>
-      <c r="D25" s="134"/>
-      <c r="E25" s="125"/>
-      <c r="F25" s="125"/>
-      <c r="G25" s="125"/>
-      <c r="H25" s="125"/>
+      <c r="A25" s="133"/>
+      <c r="B25" s="120"/>
+      <c r="C25" s="125"/>
+      <c r="D25" s="131"/>
+      <c r="E25" s="133"/>
+      <c r="F25" s="133"/>
+      <c r="G25" s="133"/>
+      <c r="H25" s="133"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
@@ -3108,10 +3108,10 @@
       <c r="B38" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="121" t="s">
+      <c r="C38" s="119" t="s">
         <v>170</v>
       </c>
-      <c r="D38" s="121" t="s">
+      <c r="D38" s="119" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3122,8 +3122,8 @@
       <c r="B39" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="123"/>
-      <c r="D39" s="123"/>
+      <c r="C39" s="120"/>
+      <c r="D39" s="120"/>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -3173,76 +3173,76 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="119"/>
-      <c r="B45" s="126" t="s">
+      <c r="A45" s="121"/>
+      <c r="B45" s="123" t="s">
         <v>166</v>
       </c>
-      <c r="C45" s="127"/>
+      <c r="C45" s="124"/>
       <c r="D45" s="31"/>
       <c r="E45" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F45" s="126" t="s">
+      <c r="F45" s="123" t="s">
         <v>16</v>
       </c>
-      <c r="G45" s="127"/>
-      <c r="H45" s="130"/>
+      <c r="G45" s="124"/>
+      <c r="H45" s="127"/>
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="120"/>
-      <c r="B46" s="128"/>
-      <c r="C46" s="129"/>
+      <c r="A46" s="122"/>
+      <c r="B46" s="125"/>
+      <c r="C46" s="126"/>
       <c r="D46" s="32"/>
       <c r="E46" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="F46" s="131"/>
-      <c r="G46" s="132"/>
-      <c r="H46" s="133"/>
+      <c r="F46" s="128"/>
+      <c r="G46" s="129"/>
+      <c r="H46" s="130"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="121" t="s">
+      <c r="A47" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="121" t="s">
+      <c r="B47" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="C47" s="126" t="s">
+      <c r="C47" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="130"/>
-      <c r="E47" s="121" t="s">
+      <c r="D47" s="127"/>
+      <c r="E47" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="F47" s="128"/>
-      <c r="G47" s="129"/>
-      <c r="H47" s="134"/>
+      <c r="F47" s="125"/>
+      <c r="G47" s="126"/>
+      <c r="H47" s="131"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="124"/>
-      <c r="B48" s="122"/>
-      <c r="C48" s="131"/>
-      <c r="D48" s="133"/>
-      <c r="E48" s="124"/>
-      <c r="F48" s="121" t="s">
+      <c r="A48" s="132"/>
+      <c r="B48" s="134"/>
+      <c r="C48" s="128"/>
+      <c r="D48" s="130"/>
+      <c r="E48" s="132"/>
+      <c r="F48" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="G48" s="121" t="s">
+      <c r="G48" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="H48" s="121" t="s">
+      <c r="H48" s="119" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="125"/>
-      <c r="B49" s="123"/>
-      <c r="C49" s="128"/>
-      <c r="D49" s="134"/>
-      <c r="E49" s="125"/>
-      <c r="F49" s="125"/>
-      <c r="G49" s="125"/>
-      <c r="H49" s="125"/>
+      <c r="A49" s="133"/>
+      <c r="B49" s="120"/>
+      <c r="C49" s="125"/>
+      <c r="D49" s="131"/>
+      <c r="E49" s="133"/>
+      <c r="F49" s="133"/>
+      <c r="G49" s="133"/>
+      <c r="H49" s="133"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
@@ -3536,10 +3536,10 @@
       <c r="B62" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C62" s="121" t="s">
+      <c r="C62" s="119" t="s">
         <v>170</v>
       </c>
-      <c r="D62" s="121" t="s">
+      <c r="D62" s="119" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3550,8 +3550,8 @@
       <c r="B63" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C63" s="123"/>
-      <c r="D63" s="123"/>
+      <c r="C63" s="120"/>
+      <c r="D63" s="120"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
@@ -3597,6 +3597,28 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="F3:H5"/>
+    <mergeCell ref="C5:D7"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="F21:H23"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
     <mergeCell ref="C62:C63"/>
     <mergeCell ref="D62:D63"/>
     <mergeCell ref="A45:A46"/>
@@ -3609,28 +3631,6 @@
     <mergeCell ref="F48:F49"/>
     <mergeCell ref="G48:G49"/>
     <mergeCell ref="H48:H49"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:C22"/>
-    <mergeCell ref="F21:H23"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="F3:H5"/>
-    <mergeCell ref="C5:D7"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="E5:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3658,18 +3658,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="126" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="134"/>
+      <c r="B1" s="126"/>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="126"/>
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="131"/>
     </row>
     <row r="2" spans="1:10" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="135" t="s">
@@ -5385,60 +5385,60 @@
       <c r="H66" s="135"/>
     </row>
     <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="121" t="s">
+      <c r="A67" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="B67" s="121" t="s">
+      <c r="B67" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="C67" s="121" t="s">
+      <c r="C67" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="D67" s="121" t="s">
+      <c r="D67" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="E67" s="121" t="s">
+      <c r="E67" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="F67" s="121" t="s">
+      <c r="F67" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="G67" s="121" t="s">
+      <c r="G67" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="H67" s="121" t="s">
+      <c r="H67" s="119" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="122"/>
-      <c r="B68" s="122"/>
-      <c r="C68" s="122"/>
-      <c r="D68" s="122"/>
-      <c r="E68" s="122"/>
-      <c r="F68" s="122"/>
-      <c r="G68" s="122"/>
-      <c r="H68" s="122"/>
+      <c r="A68" s="134"/>
+      <c r="B68" s="134"/>
+      <c r="C68" s="134"/>
+      <c r="D68" s="134"/>
+      <c r="E68" s="134"/>
+      <c r="F68" s="134"/>
+      <c r="G68" s="134"/>
+      <c r="H68" s="134"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="122"/>
-      <c r="B69" s="122"/>
-      <c r="C69" s="122"/>
-      <c r="D69" s="122"/>
-      <c r="E69" s="122"/>
-      <c r="F69" s="122"/>
-      <c r="G69" s="122"/>
-      <c r="H69" s="122"/>
+      <c r="A69" s="134"/>
+      <c r="B69" s="134"/>
+      <c r="C69" s="134"/>
+      <c r="D69" s="134"/>
+      <c r="E69" s="134"/>
+      <c r="F69" s="134"/>
+      <c r="G69" s="134"/>
+      <c r="H69" s="134"/>
     </row>
     <row r="70" spans="1:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="123"/>
-      <c r="B70" s="123"/>
-      <c r="C70" s="123"/>
-      <c r="D70" s="123"/>
-      <c r="E70" s="123"/>
-      <c r="F70" s="123"/>
-      <c r="G70" s="123"/>
-      <c r="H70" s="123"/>
+      <c r="A70" s="120"/>
+      <c r="B70" s="120"/>
+      <c r="C70" s="120"/>
+      <c r="D70" s="120"/>
+      <c r="E70" s="120"/>
+      <c r="F70" s="120"/>
+      <c r="G70" s="120"/>
+      <c r="H70" s="120"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="75">
@@ -14701,60 +14701,60 @@
       <c r="H567" s="135"/>
     </row>
     <row r="568" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A568" s="121" t="s">
+      <c r="A568" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="B568" s="121" t="s">
+      <c r="B568" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="C568" s="121" t="s">
+      <c r="C568" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="D568" s="121" t="s">
+      <c r="D568" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="E568" s="121" t="s">
+      <c r="E568" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="F568" s="121" t="s">
+      <c r="F568" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="G568" s="121" t="s">
+      <c r="G568" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="H568" s="121" t="s">
+      <c r="H568" s="119" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="569" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A569" s="122"/>
-      <c r="B569" s="122"/>
-      <c r="C569" s="122"/>
-      <c r="D569" s="122"/>
-      <c r="E569" s="122"/>
-      <c r="F569" s="122"/>
-      <c r="G569" s="122"/>
-      <c r="H569" s="122"/>
+      <c r="A569" s="134"/>
+      <c r="B569" s="134"/>
+      <c r="C569" s="134"/>
+      <c r="D569" s="134"/>
+      <c r="E569" s="134"/>
+      <c r="F569" s="134"/>
+      <c r="G569" s="134"/>
+      <c r="H569" s="134"/>
     </row>
     <row r="570" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A570" s="122"/>
-      <c r="B570" s="122"/>
-      <c r="C570" s="122"/>
-      <c r="D570" s="122"/>
-      <c r="E570" s="122"/>
-      <c r="F570" s="122"/>
-      <c r="G570" s="122"/>
-      <c r="H570" s="122"/>
+      <c r="A570" s="134"/>
+      <c r="B570" s="134"/>
+      <c r="C570" s="134"/>
+      <c r="D570" s="134"/>
+      <c r="E570" s="134"/>
+      <c r="F570" s="134"/>
+      <c r="G570" s="134"/>
+      <c r="H570" s="134"/>
     </row>
     <row r="571" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A571" s="123"/>
-      <c r="B571" s="123"/>
-      <c r="C571" s="123"/>
-      <c r="D571" s="123"/>
-      <c r="E571" s="123"/>
-      <c r="F571" s="123"/>
-      <c r="G571" s="123"/>
-      <c r="H571" s="123"/>
+      <c r="A571" s="120"/>
+      <c r="B571" s="120"/>
+      <c r="C571" s="120"/>
+      <c r="D571" s="120"/>
+      <c r="E571" s="120"/>
+      <c r="F571" s="120"/>
+      <c r="G571" s="120"/>
+      <c r="H571" s="120"/>
     </row>
     <row r="572" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A572" s="75">
@@ -16111,60 +16111,60 @@
       <c r="H626" s="135"/>
     </row>
     <row r="627" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A627" s="121" t="s">
+      <c r="A627" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="B627" s="121" t="s">
+      <c r="B627" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="C627" s="121" t="s">
+      <c r="C627" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="D627" s="121" t="s">
+      <c r="D627" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="E627" s="121" t="s">
+      <c r="E627" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="F627" s="121" t="s">
+      <c r="F627" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="G627" s="121" t="s">
+      <c r="G627" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="H627" s="121" t="s">
+      <c r="H627" s="119" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="628" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A628" s="122"/>
-      <c r="B628" s="122"/>
-      <c r="C628" s="122"/>
-      <c r="D628" s="122"/>
-      <c r="E628" s="122"/>
-      <c r="F628" s="122"/>
-      <c r="G628" s="122"/>
-      <c r="H628" s="122"/>
+      <c r="A628" s="134"/>
+      <c r="B628" s="134"/>
+      <c r="C628" s="134"/>
+      <c r="D628" s="134"/>
+      <c r="E628" s="134"/>
+      <c r="F628" s="134"/>
+      <c r="G628" s="134"/>
+      <c r="H628" s="134"/>
     </row>
     <row r="629" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A629" s="122"/>
-      <c r="B629" s="122"/>
-      <c r="C629" s="122"/>
-      <c r="D629" s="122"/>
-      <c r="E629" s="122"/>
-      <c r="F629" s="122"/>
-      <c r="G629" s="122"/>
-      <c r="H629" s="122"/>
+      <c r="A629" s="134"/>
+      <c r="B629" s="134"/>
+      <c r="C629" s="134"/>
+      <c r="D629" s="134"/>
+      <c r="E629" s="134"/>
+      <c r="F629" s="134"/>
+      <c r="G629" s="134"/>
+      <c r="H629" s="134"/>
     </row>
     <row r="630" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A630" s="123"/>
-      <c r="B630" s="123"/>
-      <c r="C630" s="123"/>
-      <c r="D630" s="123"/>
-      <c r="E630" s="123"/>
-      <c r="F630" s="123"/>
-      <c r="G630" s="123"/>
-      <c r="H630" s="123"/>
+      <c r="A630" s="120"/>
+      <c r="B630" s="120"/>
+      <c r="C630" s="120"/>
+      <c r="D630" s="120"/>
+      <c r="E630" s="120"/>
+      <c r="F630" s="120"/>
+      <c r="G630" s="120"/>
+      <c r="H630" s="120"/>
     </row>
     <row r="631" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A631" s="75">
@@ -17573,60 +17573,60 @@
       <c r="H687" s="135"/>
     </row>
     <row r="688" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A688" s="121" t="s">
+      <c r="A688" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="B688" s="121" t="s">
+      <c r="B688" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="C688" s="121" t="s">
+      <c r="C688" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="D688" s="121" t="s">
+      <c r="D688" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="E688" s="121" t="s">
+      <c r="E688" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="F688" s="121" t="s">
+      <c r="F688" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="G688" s="121" t="s">
+      <c r="G688" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="H688" s="121" t="s">
+      <c r="H688" s="119" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="689" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A689" s="122"/>
-      <c r="B689" s="122"/>
-      <c r="C689" s="122"/>
-      <c r="D689" s="122"/>
-      <c r="E689" s="122"/>
-      <c r="F689" s="122"/>
-      <c r="G689" s="122"/>
-      <c r="H689" s="122"/>
+      <c r="A689" s="134"/>
+      <c r="B689" s="134"/>
+      <c r="C689" s="134"/>
+      <c r="D689" s="134"/>
+      <c r="E689" s="134"/>
+      <c r="F689" s="134"/>
+      <c r="G689" s="134"/>
+      <c r="H689" s="134"/>
     </row>
     <row r="690" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A690" s="122"/>
-      <c r="B690" s="122"/>
-      <c r="C690" s="122"/>
-      <c r="D690" s="122"/>
-      <c r="E690" s="122"/>
-      <c r="F690" s="122"/>
-      <c r="G690" s="122"/>
-      <c r="H690" s="122"/>
+      <c r="A690" s="134"/>
+      <c r="B690" s="134"/>
+      <c r="C690" s="134"/>
+      <c r="D690" s="134"/>
+      <c r="E690" s="134"/>
+      <c r="F690" s="134"/>
+      <c r="G690" s="134"/>
+      <c r="H690" s="134"/>
     </row>
     <row r="691" spans="1:9" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A691" s="123"/>
-      <c r="B691" s="123"/>
-      <c r="C691" s="123"/>
-      <c r="D691" s="123"/>
-      <c r="E691" s="123"/>
-      <c r="F691" s="123"/>
-      <c r="G691" s="123"/>
-      <c r="H691" s="123"/>
+      <c r="A691" s="120"/>
+      <c r="B691" s="120"/>
+      <c r="C691" s="120"/>
+      <c r="D691" s="120"/>
+      <c r="E691" s="120"/>
+      <c r="F691" s="120"/>
+      <c r="G691" s="120"/>
+      <c r="H691" s="120"/>
     </row>
     <row r="692" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A692" s="75">
@@ -17891,60 +17891,60 @@
       <c r="H704" s="135"/>
     </row>
     <row r="705" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A705" s="121" t="s">
+      <c r="A705" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="B705" s="121" t="s">
+      <c r="B705" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="C705" s="121" t="s">
+      <c r="C705" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="D705" s="121" t="s">
+      <c r="D705" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="E705" s="121" t="s">
+      <c r="E705" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="F705" s="121" t="s">
+      <c r="F705" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="G705" s="121" t="s">
+      <c r="G705" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="H705" s="121" t="s">
+      <c r="H705" s="119" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="706" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A706" s="122"/>
-      <c r="B706" s="122"/>
-      <c r="C706" s="122"/>
-      <c r="D706" s="122"/>
-      <c r="E706" s="122"/>
-      <c r="F706" s="122"/>
-      <c r="G706" s="122"/>
-      <c r="H706" s="122"/>
+      <c r="A706" s="134"/>
+      <c r="B706" s="134"/>
+      <c r="C706" s="134"/>
+      <c r="D706" s="134"/>
+      <c r="E706" s="134"/>
+      <c r="F706" s="134"/>
+      <c r="G706" s="134"/>
+      <c r="H706" s="134"/>
     </row>
     <row r="707" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A707" s="122"/>
-      <c r="B707" s="122"/>
-      <c r="C707" s="122"/>
-      <c r="D707" s="122"/>
-      <c r="E707" s="122"/>
-      <c r="F707" s="122"/>
-      <c r="G707" s="122"/>
-      <c r="H707" s="122"/>
+      <c r="A707" s="134"/>
+      <c r="B707" s="134"/>
+      <c r="C707" s="134"/>
+      <c r="D707" s="134"/>
+      <c r="E707" s="134"/>
+      <c r="F707" s="134"/>
+      <c r="G707" s="134"/>
+      <c r="H707" s="134"/>
     </row>
     <row r="708" spans="1:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A708" s="123"/>
-      <c r="B708" s="123"/>
-      <c r="C708" s="123"/>
-      <c r="D708" s="123"/>
-      <c r="E708" s="123"/>
-      <c r="F708" s="123"/>
-      <c r="G708" s="123"/>
-      <c r="H708" s="123"/>
+      <c r="A708" s="120"/>
+      <c r="B708" s="120"/>
+      <c r="C708" s="120"/>
+      <c r="D708" s="120"/>
+      <c r="E708" s="120"/>
+      <c r="F708" s="120"/>
+      <c r="G708" s="120"/>
+      <c r="H708" s="120"/>
     </row>
     <row r="709" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A709" s="75">
@@ -18989,60 +18989,60 @@
       <c r="H751" s="135"/>
     </row>
     <row r="752" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A752" s="121" t="s">
+      <c r="A752" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="B752" s="121" t="s">
+      <c r="B752" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="C752" s="121" t="s">
+      <c r="C752" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="D752" s="121" t="s">
+      <c r="D752" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="E752" s="121" t="s">
+      <c r="E752" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="F752" s="121" t="s">
+      <c r="F752" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="G752" s="121" t="s">
+      <c r="G752" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="H752" s="121" t="s">
+      <c r="H752" s="119" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="753" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A753" s="122"/>
-      <c r="B753" s="122"/>
-      <c r="C753" s="122"/>
-      <c r="D753" s="122"/>
-      <c r="E753" s="122"/>
-      <c r="F753" s="122"/>
-      <c r="G753" s="122"/>
-      <c r="H753" s="122"/>
+      <c r="A753" s="134"/>
+      <c r="B753" s="134"/>
+      <c r="C753" s="134"/>
+      <c r="D753" s="134"/>
+      <c r="E753" s="134"/>
+      <c r="F753" s="134"/>
+      <c r="G753" s="134"/>
+      <c r="H753" s="134"/>
     </row>
     <row r="754" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A754" s="122"/>
-      <c r="B754" s="122"/>
-      <c r="C754" s="122"/>
-      <c r="D754" s="122"/>
-      <c r="E754" s="122"/>
-      <c r="F754" s="122"/>
-      <c r="G754" s="122"/>
-      <c r="H754" s="122"/>
+      <c r="A754" s="134"/>
+      <c r="B754" s="134"/>
+      <c r="C754" s="134"/>
+      <c r="D754" s="134"/>
+      <c r="E754" s="134"/>
+      <c r="F754" s="134"/>
+      <c r="G754" s="134"/>
+      <c r="H754" s="134"/>
     </row>
     <row r="755" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A755" s="123"/>
-      <c r="B755" s="123"/>
-      <c r="C755" s="123"/>
-      <c r="D755" s="123"/>
-      <c r="E755" s="123"/>
-      <c r="F755" s="123"/>
-      <c r="G755" s="123"/>
-      <c r="H755" s="123"/>
+      <c r="A755" s="120"/>
+      <c r="B755" s="120"/>
+      <c r="C755" s="120"/>
+      <c r="D755" s="120"/>
+      <c r="E755" s="120"/>
+      <c r="F755" s="120"/>
+      <c r="G755" s="120"/>
+      <c r="H755" s="120"/>
     </row>
     <row r="756" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A756" s="75">
@@ -21260,60 +21260,60 @@
       <c r="H865" s="135"/>
     </row>
     <row r="866" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A866" s="121" t="s">
+      <c r="A866" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="B866" s="121" t="s">
+      <c r="B866" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="C866" s="121" t="s">
+      <c r="C866" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="D866" s="121" t="s">
+      <c r="D866" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="E866" s="121" t="s">
+      <c r="E866" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="F866" s="121" t="s">
+      <c r="F866" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="G866" s="121" t="s">
+      <c r="G866" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="H866" s="121" t="s">
+      <c r="H866" s="119" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="867" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A867" s="122"/>
-      <c r="B867" s="122"/>
-      <c r="C867" s="122"/>
-      <c r="D867" s="122"/>
-      <c r="E867" s="122"/>
-      <c r="F867" s="122"/>
-      <c r="G867" s="122"/>
-      <c r="H867" s="122"/>
+      <c r="A867" s="134"/>
+      <c r="B867" s="134"/>
+      <c r="C867" s="134"/>
+      <c r="D867" s="134"/>
+      <c r="E867" s="134"/>
+      <c r="F867" s="134"/>
+      <c r="G867" s="134"/>
+      <c r="H867" s="134"/>
     </row>
     <row r="868" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A868" s="122"/>
-      <c r="B868" s="122"/>
-      <c r="C868" s="122"/>
-      <c r="D868" s="122"/>
-      <c r="E868" s="122"/>
-      <c r="F868" s="122"/>
-      <c r="G868" s="122"/>
-      <c r="H868" s="122"/>
+      <c r="A868" s="134"/>
+      <c r="B868" s="134"/>
+      <c r="C868" s="134"/>
+      <c r="D868" s="134"/>
+      <c r="E868" s="134"/>
+      <c r="F868" s="134"/>
+      <c r="G868" s="134"/>
+      <c r="H868" s="134"/>
     </row>
     <row r="869" spans="1:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A869" s="123"/>
-      <c r="B869" s="123"/>
-      <c r="C869" s="123"/>
-      <c r="D869" s="123"/>
-      <c r="E869" s="123"/>
-      <c r="F869" s="123"/>
-      <c r="G869" s="123"/>
-      <c r="H869" s="123"/>
+      <c r="A869" s="120"/>
+      <c r="B869" s="120"/>
+      <c r="C869" s="120"/>
+      <c r="D869" s="120"/>
+      <c r="E869" s="120"/>
+      <c r="F869" s="120"/>
+      <c r="G869" s="120"/>
+      <c r="H869" s="120"/>
     </row>
     <row r="870" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A870" s="75">
@@ -23141,36 +23141,55 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="A729:I729"/>
-    <mergeCell ref="A751:H751"/>
-    <mergeCell ref="A752:A755"/>
-    <mergeCell ref="B752:B755"/>
-    <mergeCell ref="C752:C755"/>
-    <mergeCell ref="D752:D755"/>
-    <mergeCell ref="E752:E755"/>
-    <mergeCell ref="F752:F755"/>
-    <mergeCell ref="G752:G755"/>
-    <mergeCell ref="H752:H755"/>
-    <mergeCell ref="A697:I697"/>
-    <mergeCell ref="A704:H704"/>
-    <mergeCell ref="A705:A708"/>
-    <mergeCell ref="B705:B708"/>
-    <mergeCell ref="C705:C708"/>
-    <mergeCell ref="D705:D708"/>
-    <mergeCell ref="E705:E708"/>
-    <mergeCell ref="F705:F708"/>
-    <mergeCell ref="G705:G708"/>
-    <mergeCell ref="H705:H708"/>
-    <mergeCell ref="A658:I658"/>
-    <mergeCell ref="A687:H687"/>
-    <mergeCell ref="A688:A691"/>
-    <mergeCell ref="B688:B691"/>
-    <mergeCell ref="C688:C691"/>
-    <mergeCell ref="D688:D691"/>
-    <mergeCell ref="E688:E691"/>
-    <mergeCell ref="F688:F691"/>
-    <mergeCell ref="G688:G691"/>
-    <mergeCell ref="H688:H691"/>
+    <mergeCell ref="F866:F869"/>
+    <mergeCell ref="G866:G869"/>
+    <mergeCell ref="H866:H869"/>
+    <mergeCell ref="A899:I899"/>
+    <mergeCell ref="A930:C930"/>
+    <mergeCell ref="A866:A869"/>
+    <mergeCell ref="B866:B869"/>
+    <mergeCell ref="C866:C869"/>
+    <mergeCell ref="D866:D869"/>
+    <mergeCell ref="E866:E869"/>
+    <mergeCell ref="A241:H241"/>
+    <mergeCell ref="A278:H278"/>
+    <mergeCell ref="A791:I791"/>
+    <mergeCell ref="A828:C828"/>
+    <mergeCell ref="A865:H865"/>
+    <mergeCell ref="A315:C315"/>
+    <mergeCell ref="A352:H352"/>
+    <mergeCell ref="A383:H383"/>
+    <mergeCell ref="A414:C414"/>
+    <mergeCell ref="A445:B445"/>
+    <mergeCell ref="A470:B470"/>
+    <mergeCell ref="A495:B495"/>
+    <mergeCell ref="A531:B531"/>
+    <mergeCell ref="A567:H567"/>
+    <mergeCell ref="A568:A571"/>
+    <mergeCell ref="B568:B571"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A52:I52"/>
+    <mergeCell ref="A66:H66"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="A127:H127"/>
+    <mergeCell ref="A157:H157"/>
+    <mergeCell ref="A187:H187"/>
+    <mergeCell ref="A214:H214"/>
+    <mergeCell ref="A59:I59"/>
+    <mergeCell ref="H67:H70"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="E67:E70"/>
+    <mergeCell ref="F67:F70"/>
+    <mergeCell ref="G67:G70"/>
+    <mergeCell ref="A98:I98"/>
     <mergeCell ref="H568:H571"/>
     <mergeCell ref="A598:I598"/>
     <mergeCell ref="A626:H626"/>
@@ -23187,55 +23206,36 @@
     <mergeCell ref="E568:E571"/>
     <mergeCell ref="F568:F571"/>
     <mergeCell ref="G568:G571"/>
-    <mergeCell ref="A127:H127"/>
-    <mergeCell ref="A157:H157"/>
-    <mergeCell ref="A187:H187"/>
-    <mergeCell ref="A214:H214"/>
-    <mergeCell ref="A59:I59"/>
-    <mergeCell ref="H67:H70"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="D67:D70"/>
-    <mergeCell ref="E67:E70"/>
-    <mergeCell ref="F67:F70"/>
-    <mergeCell ref="G67:G70"/>
-    <mergeCell ref="A98:I98"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A52:I52"/>
-    <mergeCell ref="A66:H66"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A14:J14"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="A34:J34"/>
-    <mergeCell ref="A241:H241"/>
-    <mergeCell ref="A278:H278"/>
-    <mergeCell ref="A791:I791"/>
-    <mergeCell ref="A828:C828"/>
-    <mergeCell ref="A865:H865"/>
-    <mergeCell ref="A315:C315"/>
-    <mergeCell ref="A352:H352"/>
-    <mergeCell ref="A383:H383"/>
-    <mergeCell ref="A414:C414"/>
-    <mergeCell ref="A445:B445"/>
-    <mergeCell ref="A470:B470"/>
-    <mergeCell ref="A495:B495"/>
-    <mergeCell ref="A531:B531"/>
-    <mergeCell ref="A567:H567"/>
-    <mergeCell ref="A568:A571"/>
-    <mergeCell ref="B568:B571"/>
-    <mergeCell ref="F866:F869"/>
-    <mergeCell ref="G866:G869"/>
-    <mergeCell ref="H866:H869"/>
-    <mergeCell ref="A899:I899"/>
-    <mergeCell ref="A930:C930"/>
-    <mergeCell ref="A866:A869"/>
-    <mergeCell ref="B866:B869"/>
-    <mergeCell ref="C866:C869"/>
-    <mergeCell ref="D866:D869"/>
-    <mergeCell ref="E866:E869"/>
+    <mergeCell ref="A658:I658"/>
+    <mergeCell ref="A687:H687"/>
+    <mergeCell ref="A688:A691"/>
+    <mergeCell ref="B688:B691"/>
+    <mergeCell ref="C688:C691"/>
+    <mergeCell ref="D688:D691"/>
+    <mergeCell ref="E688:E691"/>
+    <mergeCell ref="F688:F691"/>
+    <mergeCell ref="G688:G691"/>
+    <mergeCell ref="H688:H691"/>
+    <mergeCell ref="A697:I697"/>
+    <mergeCell ref="A704:H704"/>
+    <mergeCell ref="A705:A708"/>
+    <mergeCell ref="B705:B708"/>
+    <mergeCell ref="C705:C708"/>
+    <mergeCell ref="D705:D708"/>
+    <mergeCell ref="E705:E708"/>
+    <mergeCell ref="F705:F708"/>
+    <mergeCell ref="G705:G708"/>
+    <mergeCell ref="H705:H708"/>
+    <mergeCell ref="A729:I729"/>
+    <mergeCell ref="A751:H751"/>
+    <mergeCell ref="A752:A755"/>
+    <mergeCell ref="B752:B755"/>
+    <mergeCell ref="C752:C755"/>
+    <mergeCell ref="D752:D755"/>
+    <mergeCell ref="E752:E755"/>
+    <mergeCell ref="F752:F755"/>
+    <mergeCell ref="G752:G755"/>
+    <mergeCell ref="H752:H755"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23916,7 +23916,7 @@
       <c r="G35" s="135"/>
       <c r="H35" s="135"/>
       <c r="I35" s="136"/>
-      <c r="J35" s="121" t="s">
+      <c r="J35" s="119" t="s">
         <v>92</v>
       </c>
     </row>
@@ -23948,7 +23948,7 @@
       <c r="I36" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="J36" s="123"/>
+      <c r="J36" s="120"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
@@ -24000,7 +24000,7 @@
       <c r="G40" s="135"/>
       <c r="H40" s="135"/>
       <c r="I40" s="136"/>
-      <c r="J40" s="121" t="s">
+      <c r="J40" s="119" t="s">
         <v>95</v>
       </c>
     </row>
@@ -24032,7 +24032,7 @@
       <c r="I41" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="J41" s="123"/>
+      <c r="J41" s="120"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="28" t="s">
@@ -24626,7 +24626,7 @@
       <c r="G90" s="135"/>
       <c r="H90" s="135"/>
       <c r="I90" s="136"/>
-      <c r="J90" s="121" t="s">
+      <c r="J90" s="119" t="s">
         <v>92</v>
       </c>
     </row>
@@ -24658,7 +24658,7 @@
       <c r="I91" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="J91" s="123"/>
+      <c r="J91" s="120"/>
     </row>
     <row r="92" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="28" t="s">
@@ -24710,7 +24710,7 @@
       <c r="G95" s="135"/>
       <c r="H95" s="135"/>
       <c r="I95" s="136"/>
-      <c r="J95" s="121" t="s">
+      <c r="J95" s="119" t="s">
         <v>95</v>
       </c>
     </row>
@@ -24742,7 +24742,7 @@
       <c r="I96" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="J96" s="123"/>
+      <c r="J96" s="120"/>
     </row>
     <row r="97" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="28" t="s">
@@ -24951,10 +24951,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25677,7 +25677,7 @@
         <v>-719.1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="28" t="s">
         <v>51</v>
       </c>
@@ -25694,7 +25694,7 @@
         <v>1126.3</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="28" t="s">
         <v>235</v>
       </c>
@@ -25707,12 +25707,11 @@
       <c r="D50" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E50" s="47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="28" t="s">
         <v>120</v>
       </c>
@@ -25729,7 +25728,7 @@
         <v>-9422.4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="28" t="s">
         <v>121</v>
       </c>
@@ -25746,7 +25745,7 @@
         <v>267060.59999999998</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="28" t="s">
         <v>122</v>
       </c>
@@ -25763,12 +25762,12 @@
         <v>267060.59999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="139" t="s">
         <v>109</v>
       </c>
@@ -25777,7 +25776,7 @@
       <c r="D56" s="135"/>
       <c r="E56" s="136"/>
     </row>
-    <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="139" t="s">
         <v>110</v>
       </c>
@@ -25786,7 +25785,7 @@
       <c r="D57" s="135"/>
       <c r="E57" s="136"/>
     </row>
-    <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="28"/>
       <c r="B58" s="28" t="s">
         <v>26</v>
@@ -25801,7 +25800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="41.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="28" t="s">
         <v>112</v>
       </c>
@@ -25818,12 +25817,12 @@
         <v>63856.6</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="28" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="28" t="s">
         <v>114</v>
       </c>
@@ -25840,7 +25839,7 @@
         <v>1301.3</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="28" t="s">
         <v>20</v>
       </c>
@@ -25857,7 +25856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="28" t="s">
         <v>115</v>
       </c>
@@ -25874,7 +25873,7 @@
         <v>271.3</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="28" t="s">
         <v>116</v>
       </c>
@@ -27198,13 +27197,6 @@
     <row r="72" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="G2:H2"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="D42:F42"/>
@@ -27218,6 +27210,13 @@
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="G22:H22"/>
     <mergeCell ref="A31:H31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27533,7 +27532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>